<commit_message>
unlocked secrets of R^I ligatures and the code point 161
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="858">
   <si>
     <t>' r underbar</t>
   </si>
@@ -2586,6 +2586,18 @@
   </si>
   <si>
     <t>Java Test Template</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>manually added to sanskrit99 conversion</t>
+  </si>
+  <si>
+    <t>same in both, conversion not needed</t>
+  </si>
+  <si>
+    <t>already present and uses special logic for conversion because of placement</t>
   </si>
 </sst>
 </file>
@@ -2701,13 +2713,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2721,8 +2733,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1139">
+  <cellStyleXfs count="1153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3897,10 +3923,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1139">
+  <cellStyles count="1153">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4470,6 +4496,13 @@
     <cellStyle name="Followed Hyperlink" xfId="1134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1152" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5039,17 +5072,16 @@
     <cellStyle name="Hyperlink" xfId="1133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1151" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6740,10 +6772,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:H207"/>
+  <dimension ref="A1:H213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6781,7 +6813,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8">
       <c r="A2">
         <f>HEX2DEC(MID(B2,3,4))</f>
         <v>50</v>
@@ -6803,11 +6835,11 @@
         <v>\x32</v>
       </c>
       <c r="H2" s="14" t="str">
-        <f t="shared" ref="H1:H64" si="0">CONCATENATE("@Test public void testConvert_",A2,"() throws Exception { verify( (char) ",A2, ", """,C2,"""); }")</f>
+        <f t="shared" ref="H2:H64" si="0">CONCATENATE("@Test public void testConvert_",A2,"() throws Exception { verify( (char) ",A2, ", """,C2,"""); }")</f>
         <v>@Test public void testConvert_50() throws Exception { verify( (char) 50, "2"); }</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="1">HEX2DEC(MID(B3,3,4))</f>
         <v>51</v>
@@ -6833,7 +6865,7 @@
         <v>@Test public void testConvert_51() throws Exception { verify( (char) 51, "3"); }</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -6859,7 +6891,7 @@
         <v>@Test public void testConvert_52() throws Exception { verify( (char) 52, "4"); }</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -6885,7 +6917,7 @@
         <v>@Test public void testConvert_53() throws Exception { verify( (char) 53, "5"); }</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -6911,7 +6943,7 @@
         <v>@Test public void testConvert_54() throws Exception { verify( (char) 54, "6"); }</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -6937,7 +6969,7 @@
         <v>@Test public void testConvert_55() throws Exception { verify( (char) 55, "7"); }</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -6963,7 +6995,7 @@
         <v>@Test public void testConvert_56() throws Exception { verify( (char) 56, "8"); }</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -6989,7 +7021,7 @@
         <v>@Test public void testConvert_57() throws Exception { verify( (char) 57, "9"); }</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -7015,7 +7047,7 @@
         <v>@Test public void testConvert_58() throws Exception { verify( (char) 58, ":"); }</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -7041,7 +7073,7 @@
         <v>@Test public void testConvert_59() throws Exception { verify( (char) 59, ";"); }</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -7067,7 +7099,7 @@
         <v>@Test public void testConvert_60() throws Exception { verify( (char) 60, "&lt;"); }</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -7093,7 +7125,7 @@
         <v>@Test public void testConvert_61() throws Exception { verify( (char) 61, "="); }</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -7119,7 +7151,7 @@
         <v>@Test public void testConvert_62() throws Exception { verify( (char) 62, "&gt;"); }</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -7145,7 +7177,7 @@
         <v>@Test public void testConvert_63() throws Exception { verify( (char) 63, "?"); }</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -7171,7 +7203,7 @@
         <v>@Test public void testConvert_64() throws Exception { verify( (char) 64, "@"); }</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -7197,7 +7229,7 @@
         <v>@Test public void testConvert_65() throws Exception { verify( (char) 65, "A"); }</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:8">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -7223,7 +7255,7 @@
         <v>@Test public void testConvert_66() throws Exception { verify( (char) 66, "B"); }</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:8">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -7249,7 +7281,7 @@
         <v>@Test public void testConvert_67() throws Exception { verify( (char) 67, "C"); }</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:8">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -7275,7 +7307,7 @@
         <v>@Test public void testConvert_68() throws Exception { verify( (char) 68, "D"); }</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1">
+    <row r="21" spans="1:8">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -7301,7 +7333,7 @@
         <v>@Test public void testConvert_69() throws Exception { verify( (char) 69, "E"); }</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1">
+    <row r="22" spans="1:8">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -7327,7 +7359,7 @@
         <v>@Test public void testConvert_70() throws Exception { verify( (char) 70, "F"); }</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1">
+    <row r="23" spans="1:8">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -7353,7 +7385,7 @@
         <v>@Test public void testConvert_71() throws Exception { verify( (char) 71, "G"); }</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1">
+    <row r="24" spans="1:8">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -7379,7 +7411,7 @@
         <v>@Test public void testConvert_72() throws Exception { verify( (char) 72, "H"); }</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1">
+    <row r="25" spans="1:8">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -7405,7 +7437,7 @@
         <v>@Test public void testConvert_73() throws Exception { verify( (char) 73, "I"); }</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1">
+    <row r="26" spans="1:8">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -7431,7 +7463,7 @@
         <v>@Test public void testConvert_74() throws Exception { verify( (char) 74, "J"); }</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1">
+    <row r="27" spans="1:8">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -7457,7 +7489,7 @@
         <v>@Test public void testConvert_75() throws Exception { verify( (char) 75, "K"); }</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1">
+    <row r="28" spans="1:8">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -7483,7 +7515,7 @@
         <v>@Test public void testConvert_76() throws Exception { verify( (char) 76, "L"); }</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1">
+    <row r="29" spans="1:8">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -7509,7 +7541,7 @@
         <v>@Test public void testConvert_77() throws Exception { verify( (char) 77, "M"); }</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1">
+    <row r="30" spans="1:8">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -7535,7 +7567,7 @@
         <v>@Test public void testConvert_78() throws Exception { verify( (char) 78, "N"); }</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1">
+    <row r="31" spans="1:8">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -7561,7 +7593,7 @@
         <v>@Test public void testConvert_79() throws Exception { verify( (char) 79, "O"); }</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1">
+    <row r="32" spans="1:8">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -7587,7 +7619,7 @@
         <v>@Test public void testConvert_80() throws Exception { verify( (char) 80, "P"); }</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1">
+    <row r="33" spans="1:8">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -7621,7 +7653,7 @@
       <c r="B34" t="s">
         <v>284</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="28" t="s">
         <v>285</v>
       </c>
       <c r="D34">
@@ -7639,7 +7671,7 @@
         <v>@Test public void testConvert_82() throws Exception { verify( (char) 82, "R"); }</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -7665,7 +7697,7 @@
         <v>@Test public void testConvert_83() throws Exception { verify( (char) 83, "S"); }</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -7691,7 +7723,7 @@
         <v>@Test public void testConvert_84() throws Exception { verify( (char) 84, "T"); }</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -7717,7 +7749,7 @@
         <v>@Test public void testConvert_85() throws Exception { verify( (char) 85, "U"); }</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -7743,7 +7775,7 @@
         <v>@Test public void testConvert_86() throws Exception { verify( (char) 86, "V"); }</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -7769,7 +7801,7 @@
         <v>@Test public void testConvert_87() throws Exception { verify( (char) 87, "W"); }</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -7795,7 +7827,7 @@
         <v>@Test public void testConvert_88() throws Exception { verify( (char) 88, "X"); }</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -7821,7 +7853,7 @@
         <v>@Test public void testConvert_89() throws Exception { verify( (char) 89, "Y"); }</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -7847,7 +7879,7 @@
         <v>@Test public void testConvert_90() throws Exception { verify( (char) 90, "Z"); }</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -7873,7 +7905,7 @@
         <v>@Test public void testConvert_91() throws Exception { verify( (char) 91, "["); }</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1">
+    <row r="44" spans="1:8">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -7899,7 +7931,7 @@
         <v>@Test public void testConvert_92() throws Exception { verify( (char) 92, "\"); }</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1">
+    <row r="45" spans="1:8">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -7925,7 +7957,7 @@
         <v>@Test public void testConvert_93() throws Exception { verify( (char) 93, "]"); }</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1">
+    <row r="46" spans="1:8">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -7951,7 +7983,7 @@
         <v>@Test public void testConvert_94() throws Exception { verify( (char) 94, "^"); }</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1">
+    <row r="47" spans="1:8">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -7977,7 +8009,7 @@
         <v>@Test public void testConvert_95() throws Exception { verify( (char) 95, "_"); }</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1">
+    <row r="48" spans="1:8">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -8003,7 +8035,7 @@
         <v>@Test public void testConvert_96() throws Exception { verify( (char) 96, "`"); }</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1">
+    <row r="49" spans="1:8">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -8029,7 +8061,7 @@
         <v>@Test public void testConvert_97() throws Exception { verify( (char) 97, "a"); }</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1">
+    <row r="50" spans="1:8">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -8055,7 +8087,7 @@
         <v>@Test public void testConvert_98() throws Exception { verify( (char) 98, "b"); }</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1">
+    <row r="51" spans="1:8">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -8081,7 +8113,7 @@
         <v>@Test public void testConvert_99() throws Exception { verify( (char) 99, "c"); }</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1">
+    <row r="52" spans="1:8">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -8107,7 +8139,7 @@
         <v>@Test public void testConvert_100() throws Exception { verify( (char) 100, "d"); }</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1">
+    <row r="53" spans="1:8">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -8133,7 +8165,7 @@
         <v>@Test public void testConvert_101() throws Exception { verify( (char) 101, "e"); }</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1">
+    <row r="54" spans="1:8">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -8159,7 +8191,7 @@
         <v>@Test public void testConvert_102() throws Exception { verify( (char) 102, "f"); }</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1">
+    <row r="55" spans="1:8">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -8185,7 +8217,7 @@
         <v>@Test public void testConvert_103() throws Exception { verify( (char) 103, "g"); }</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1">
+    <row r="56" spans="1:8">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -8219,7 +8251,7 @@
       <c r="B57" t="s">
         <v>359</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="28" t="s">
         <v>360</v>
       </c>
       <c r="D57">
@@ -8237,7 +8269,7 @@
         <v>@Test public void testConvert_105() throws Exception { verify( (char) 105, "i"); }</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1">
+    <row r="58" spans="1:8">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -8263,7 +8295,7 @@
         <v>@Test public void testConvert_106() throws Exception { verify( (char) 106, "j"); }</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1">
+    <row r="59" spans="1:8">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -8289,7 +8321,7 @@
         <v>@Test public void testConvert_107() throws Exception { verify( (char) 107, "k"); }</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1">
+    <row r="60" spans="1:8">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -8315,7 +8347,7 @@
         <v>@Test public void testConvert_108() throws Exception { verify( (char) 108, "l"); }</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1">
+    <row r="61" spans="1:8">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -8341,7 +8373,7 @@
         <v>@Test public void testConvert_109() throws Exception { verify( (char) 109, "m"); }</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:8">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -8367,7 +8399,7 @@
         <v>@Test public void testConvert_110() throws Exception { verify( (char) 110, "n"); }</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1">
+    <row r="63" spans="1:8">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -8393,7 +8425,7 @@
         <v>@Test public void testConvert_111() throws Exception { verify( (char) 111, "o"); }</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1">
+    <row r="64" spans="1:8">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -8419,7 +8451,7 @@
         <v>@Test public void testConvert_112() throws Exception { verify( (char) 112, "p"); }</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1">
+    <row r="65" spans="1:8">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -8445,7 +8477,7 @@
         <v>@Test public void testConvert_113() throws Exception { verify( (char) 113, "q"); }</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1">
+    <row r="66" spans="1:8">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -8471,7 +8503,7 @@
         <v>@Test public void testConvert_114() throws Exception { verify( (char) 114, "r"); }</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1">
+    <row r="67" spans="1:8">
       <c r="A67">
         <f t="shared" ref="A67:A78" si="4">HEX2DEC(MID(B67,3,4))</f>
         <v>115</v>
@@ -8497,7 +8529,7 @@
         <v>@Test public void testConvert_115() throws Exception { verify( (char) 115, "s"); }</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1">
+    <row r="68" spans="1:8">
       <c r="A68">
         <f t="shared" si="4"/>
         <v>116</v>
@@ -8523,7 +8555,7 @@
         <v>@Test public void testConvert_116() throws Exception { verify( (char) 116, "t"); }</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1">
+    <row r="69" spans="1:8">
       <c r="A69">
         <f t="shared" si="4"/>
         <v>117</v>
@@ -8549,7 +8581,7 @@
         <v>@Test public void testConvert_117() throws Exception { verify( (char) 117, "u"); }</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1">
+    <row r="70" spans="1:8">
       <c r="A70">
         <f t="shared" si="4"/>
         <v>118</v>
@@ -8575,7 +8607,7 @@
         <v>@Test public void testConvert_118() throws Exception { verify( (char) 118, "v"); }</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1">
+    <row r="71" spans="1:8">
       <c r="A71">
         <f t="shared" si="4"/>
         <v>119</v>
@@ -8601,7 +8633,7 @@
         <v>@Test public void testConvert_119() throws Exception { verify( (char) 119, "w"); }</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1">
+    <row r="72" spans="1:8">
       <c r="A72">
         <f t="shared" si="4"/>
         <v>120</v>
@@ -8627,7 +8659,7 @@
         <v>@Test public void testConvert_120() throws Exception { verify( (char) 120, "x"); }</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1">
+    <row r="73" spans="1:8">
       <c r="A73">
         <f t="shared" si="4"/>
         <v>121</v>
@@ -8653,7 +8685,7 @@
         <v>@Test public void testConvert_121() throws Exception { verify( (char) 121, "y"); }</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1">
+    <row r="74" spans="1:8">
       <c r="A74">
         <f t="shared" si="4"/>
         <v>122</v>
@@ -8679,7 +8711,7 @@
         <v>@Test public void testConvert_122() throws Exception { verify( (char) 122, "z"); }</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1">
+    <row r="75" spans="1:8">
       <c r="A75">
         <f t="shared" si="4"/>
         <v>123</v>
@@ -8705,7 +8737,7 @@
         <v>@Test public void testConvert_123() throws Exception { verify( (char) 123, "{"); }</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1">
+    <row r="76" spans="1:8">
       <c r="A76">
         <f t="shared" si="4"/>
         <v>124</v>
@@ -8731,7 +8763,7 @@
         <v>@Test public void testConvert_124() throws Exception { verify( (char) 124, "|"); }</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1">
+    <row r="77" spans="1:8">
       <c r="A77">
         <f t="shared" si="4"/>
         <v>125</v>
@@ -8757,7 +8789,7 @@
         <v>@Test public void testConvert_125() throws Exception { verify( (char) 125, "}"); }</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1">
+    <row r="78" spans="1:8">
       <c r="A78">
         <f t="shared" si="4"/>
         <v>126</v>
@@ -8828,7 +8860,7 @@
         <v>\xc2\x81</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1">
+    <row r="82" spans="1:8">
       <c r="A82">
         <f t="shared" ref="A82:A92" si="7">HEX2DEC(MID(B82,3,4))</f>
         <v>130</v>
@@ -8851,7 +8883,7 @@
         <v>@Test public void testConvert_130() throws Exception { verify( (char) 130, ""); }</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1">
+    <row r="83" spans="1:8">
       <c r="A83">
         <f t="shared" si="7"/>
         <v>131</v>
@@ -8874,7 +8906,7 @@
         <v>@Test public void testConvert_131() throws Exception { verify( (char) 131, ""); }</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1">
+    <row r="84" spans="1:8">
       <c r="A84">
         <f t="shared" si="7"/>
         <v>132</v>
@@ -8897,7 +8929,7 @@
         <v>@Test public void testConvert_132() throws Exception { verify( (char) 132, ""); }</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1">
+    <row r="85" spans="1:8">
       <c r="A85">
         <f t="shared" si="7"/>
         <v>133</v>
@@ -8920,7 +8952,7 @@
         <v>@Test public void testConvert_133() throws Exception { verify( (char) 133, ""); }</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1">
+    <row r="86" spans="1:8">
       <c r="A86">
         <f t="shared" si="7"/>
         <v>134</v>
@@ -8943,7 +8975,7 @@
         <v>@Test public void testConvert_134() throws Exception { verify( (char) 134, ""); }</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1">
+    <row r="87" spans="1:8">
       <c r="A87">
         <f t="shared" si="7"/>
         <v>135</v>
@@ -8966,7 +8998,7 @@
         <v>@Test public void testConvert_135() throws Exception { verify( (char) 135, ""); }</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1">
+    <row r="88" spans="1:8">
       <c r="A88">
         <f t="shared" si="7"/>
         <v>136</v>
@@ -8989,7 +9021,7 @@
         <v>@Test public void testConvert_136() throws Exception { verify( (char) 136, ""); }</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1">
+    <row r="89" spans="1:8">
       <c r="A89">
         <f t="shared" si="7"/>
         <v>137</v>
@@ -9012,7 +9044,7 @@
         <v>@Test public void testConvert_137() throws Exception { verify( (char) 137, ""); }</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1">
+    <row r="90" spans="1:8">
       <c r="A90">
         <f t="shared" si="7"/>
         <v>138</v>
@@ -9035,7 +9067,7 @@
         <v>@Test public void testConvert_138() throws Exception { verify( (char) 138, ""); }</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1">
+    <row r="91" spans="1:8">
       <c r="A91">
         <f t="shared" si="7"/>
         <v>139</v>
@@ -9058,7 +9090,7 @@
         <v>@Test public void testConvert_139() throws Exception { verify( (char) 139, ""); }</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1">
+    <row r="92" spans="1:8">
       <c r="A92">
         <f t="shared" si="7"/>
         <v>140</v>
@@ -9141,7 +9173,7 @@
         <v>\xc2\x90</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1">
+    <row r="97" spans="1:8">
       <c r="A97">
         <f t="shared" ref="A97:A108" si="9">HEX2DEC(MID(B97,3,4))</f>
         <v>145</v>
@@ -9164,7 +9196,7 @@
         <v>@Test public void testConvert_145() throws Exception { verify( (char) 145, ""); }</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1">
+    <row r="98" spans="1:8">
       <c r="A98">
         <f t="shared" si="9"/>
         <v>146</v>
@@ -9187,7 +9219,7 @@
         <v>@Test public void testConvert_146() throws Exception { verify( (char) 146, ""); }</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1">
+    <row r="99" spans="1:8">
       <c r="A99">
         <f t="shared" si="9"/>
         <v>147</v>
@@ -9210,7 +9242,7 @@
         <v>@Test public void testConvert_147() throws Exception { verify( (char) 147, ""); }</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1">
+    <row r="100" spans="1:8">
       <c r="A100">
         <f t="shared" si="9"/>
         <v>148</v>
@@ -9233,7 +9265,7 @@
         <v>@Test public void testConvert_148() throws Exception { verify( (char) 148, ""); }</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1">
+    <row r="101" spans="1:8">
       <c r="A101">
         <f t="shared" si="9"/>
         <v>149</v>
@@ -9256,7 +9288,7 @@
         <v>@Test public void testConvert_149() throws Exception { verify( (char) 149, ""); }</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1">
+    <row r="102" spans="1:8">
       <c r="A102">
         <f t="shared" si="9"/>
         <v>150</v>
@@ -9279,7 +9311,7 @@
         <v>@Test public void testConvert_150() throws Exception { verify( (char) 150, ""); }</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1">
+    <row r="103" spans="1:8">
       <c r="A103">
         <f t="shared" si="9"/>
         <v>151</v>
@@ -9302,7 +9334,7 @@
         <v>@Test public void testConvert_151() throws Exception { verify( (char) 151, ""); }</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1">
+    <row r="104" spans="1:8">
       <c r="A104">
         <f t="shared" si="9"/>
         <v>152</v>
@@ -9325,7 +9357,7 @@
         <v>@Test public void testConvert_152() throws Exception { verify( (char) 152, ""); }</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1">
+    <row r="105" spans="1:8">
       <c r="A105">
         <f t="shared" si="9"/>
         <v>153</v>
@@ -9348,7 +9380,7 @@
         <v>@Test public void testConvert_153() throws Exception { verify( (char) 153, ""); }</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1">
+    <row r="106" spans="1:8">
       <c r="A106">
         <f t="shared" si="9"/>
         <v>154</v>
@@ -9371,7 +9403,7 @@
         <v>@Test public void testConvert_154() throws Exception { verify( (char) 154, ""); }</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1">
+    <row r="107" spans="1:8">
       <c r="A107">
         <f t="shared" si="9"/>
         <v>155</v>
@@ -9394,7 +9426,7 @@
         <v>@Test public void testConvert_155() throws Exception { verify( (char) 155, ""); }</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1">
+    <row r="108" spans="1:8">
       <c r="A108">
         <f t="shared" si="9"/>
         <v>156</v>
@@ -9447,7 +9479,7 @@
         <v>\xc2\x9e</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1">
+    <row r="111" spans="1:8">
       <c r="A111">
         <f t="shared" ref="A111:A174" si="11">HEX2DEC(MID(B111,3,4))</f>
         <v>159</v>
@@ -9470,7 +9502,7 @@
         <v>@Test public void testConvert_159() throws Exception { verify( (char) 159, ""); }</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1">
+    <row r="112" spans="1:8">
       <c r="A112">
         <f t="shared" si="11"/>
         <v>160</v>
@@ -9519,7 +9551,7 @@
         <v>@Test public void testConvert_161() throws Exception { verify( (char) 161, "¡"); }</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1">
+    <row r="114" spans="1:8">
       <c r="A114">
         <f t="shared" si="11"/>
         <v>162</v>
@@ -9545,7 +9577,7 @@
         <v>@Test public void testConvert_162() throws Exception { verify( (char) 162, "¢"); }</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1">
+    <row r="115" spans="1:8">
       <c r="A115">
         <f t="shared" si="11"/>
         <v>163</v>
@@ -9571,7 +9603,7 @@
         <v>@Test public void testConvert_163() throws Exception { verify( (char) 163, "£"); }</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1">
+    <row r="116" spans="1:8">
       <c r="A116">
         <f t="shared" si="11"/>
         <v>164</v>
@@ -9597,7 +9629,7 @@
         <v>@Test public void testConvert_164() throws Exception { verify( (char) 164, "¤"); }</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1">
+    <row r="117" spans="1:8">
       <c r="A117">
         <f t="shared" si="11"/>
         <v>165</v>
@@ -9623,7 +9655,7 @@
         <v>@Test public void testConvert_165() throws Exception { verify( (char) 165, "¥"); }</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1">
+    <row r="118" spans="1:8">
       <c r="A118">
         <f t="shared" si="11"/>
         <v>166</v>
@@ -9649,7 +9681,7 @@
         <v>@Test public void testConvert_166() throws Exception { verify( (char) 166, "¦"); }</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1">
+    <row r="119" spans="1:8">
       <c r="A119">
         <f t="shared" si="11"/>
         <v>167</v>
@@ -9675,7 +9707,7 @@
         <v>@Test public void testConvert_167() throws Exception { verify( (char) 167, "§"); }</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1">
+    <row r="120" spans="1:8">
       <c r="A120">
         <f t="shared" si="11"/>
         <v>168</v>
@@ -9696,12 +9728,12 @@
         <f t="shared" si="6"/>
         <v>\xc2\xa8</v>
       </c>
-      <c r="H120" s="14" t="str">
+      <c r="H120" s="25" t="str">
         <f t="shared" si="12"/>
         <v>@Test public void testConvert_168() throws Exception { verify( (char) 168, "¨"); }</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1">
+    <row r="121" spans="1:8">
       <c r="A121">
         <f t="shared" si="11"/>
         <v>169</v>
@@ -9722,12 +9754,12 @@
         <f t="shared" si="6"/>
         <v>\xc2\xa9</v>
       </c>
-      <c r="H121" s="14" t="str">
+      <c r="H121" s="25" t="str">
         <f t="shared" si="12"/>
         <v>@Test public void testConvert_169() throws Exception { verify( (char) 169, "©"); }</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1">
+    <row r="122" spans="1:8">
       <c r="A122">
         <f t="shared" si="11"/>
         <v>170</v>
@@ -9753,7 +9785,7 @@
         <v>@Test public void testConvert_170() throws Exception { verify( (char) 170, "ª"); }</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1">
+    <row r="123" spans="1:8">
       <c r="A123">
         <f t="shared" si="11"/>
         <v>171</v>
@@ -9779,7 +9811,7 @@
         <v>@Test public void testConvert_171() throws Exception { verify( (char) 171, "«"); }</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1">
+    <row r="124" spans="1:8">
       <c r="A124">
         <f t="shared" si="11"/>
         <v>172</v>
@@ -9810,10 +9842,10 @@
         <f t="shared" si="11"/>
         <v>173</v>
       </c>
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="20" t="s">
         <v>553</v>
       </c>
-      <c r="C125" s="26"/>
+      <c r="C125" s="29"/>
       <c r="D125" t="s">
         <v>554</v>
       </c>
@@ -9832,7 +9864,7 @@
         <v>@Test public void testConvert_173() throws Exception { verify( (char) 173, ""); }</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1">
+    <row r="126" spans="1:8">
       <c r="A126">
         <f t="shared" si="11"/>
         <v>174</v>
@@ -9858,7 +9890,7 @@
         <v>@Test public void testConvert_174() throws Exception { verify( (char) 174, "®"); }</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1">
+    <row r="127" spans="1:8">
       <c r="A127">
         <f t="shared" si="11"/>
         <v>175</v>
@@ -9962,7 +9994,7 @@
         <v>@Test public void testConvert_178() throws Exception { verify( (char) 178, "²"); }</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1">
+    <row r="131" spans="1:8">
       <c r="A131">
         <f t="shared" si="11"/>
         <v>179</v>
@@ -9988,7 +10020,7 @@
         <v>@Test public void testConvert_179() throws Exception { verify( (char) 179, "³"); }</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1">
+    <row r="132" spans="1:8">
       <c r="A132">
         <f t="shared" si="11"/>
         <v>180</v>
@@ -10014,7 +10046,7 @@
         <v>@Test public void testConvert_180() throws Exception { verify( (char) 180, "´"); }</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1">
+    <row r="133" spans="1:8">
       <c r="A133">
         <f t="shared" si="11"/>
         <v>181</v>
@@ -10040,7 +10072,7 @@
         <v>@Test public void testConvert_181() throws Exception { verify( (char) 181, "µ"); }</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1">
+    <row r="134" spans="1:8">
       <c r="A134">
         <f t="shared" si="11"/>
         <v>182</v>
@@ -10074,7 +10106,7 @@
       <c r="B135" t="s">
         <v>592</v>
       </c>
-      <c r="C135" s="26" t="s">
+      <c r="C135" s="29" t="s">
         <v>593</v>
       </c>
       <c r="D135" t="s">
@@ -10095,7 +10127,7 @@
         <v>@Test public void testConvert_183() throws Exception { verify( (char) 183, "·"); }</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1">
+    <row r="136" spans="1:8">
       <c r="A136">
         <f t="shared" si="11"/>
         <v>184</v>
@@ -10121,7 +10153,7 @@
         <v>@Test public void testConvert_184() throws Exception { verify( (char) 184, "¸"); }</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1">
+    <row r="137" spans="1:8">
       <c r="A137">
         <f t="shared" si="11"/>
         <v>185</v>
@@ -10147,7 +10179,7 @@
         <v>@Test public void testConvert_185() throws Exception { verify( (char) 185, "¹"); }</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1">
+    <row r="138" spans="1:8">
       <c r="A138">
         <f t="shared" si="11"/>
         <v>186</v>
@@ -10173,7 +10205,7 @@
         <v>@Test public void testConvert_186() throws Exception { verify( (char) 186, "º"); }</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1">
+    <row r="139" spans="1:8">
       <c r="A139">
         <f t="shared" si="11"/>
         <v>187</v>
@@ -10199,7 +10231,7 @@
         <v>@Test public void testConvert_187() throws Exception { verify( (char) 187, "»"); }</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1">
+    <row r="140" spans="1:8">
       <c r="A140">
         <f t="shared" si="11"/>
         <v>188</v>
@@ -10225,7 +10257,7 @@
         <v>@Test public void testConvert_188() throws Exception { verify( (char) 188, "¼"); }</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1">
+    <row r="141" spans="1:8">
       <c r="A141">
         <f t="shared" si="11"/>
         <v>189</v>
@@ -10251,7 +10283,7 @@
         <v>@Test public void testConvert_189() throws Exception { verify( (char) 189, "½"); }</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1">
+    <row r="142" spans="1:8">
       <c r="A142">
         <f t="shared" si="11"/>
         <v>190</v>
@@ -10277,7 +10309,7 @@
         <v>@Test public void testConvert_190() throws Exception { verify( (char) 190, "¾"); }</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1">
+    <row r="143" spans="1:8">
       <c r="A143">
         <f t="shared" si="11"/>
         <v>191</v>
@@ -10303,7 +10335,7 @@
         <v>@Test public void testConvert_191() throws Exception { verify( (char) 191, "¿"); }</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1">
+    <row r="144" spans="1:8">
       <c r="A144">
         <f t="shared" si="11"/>
         <v>192</v>
@@ -10329,7 +10361,7 @@
         <v>@Test public void testConvert_192() throws Exception { verify( (char) 192, "À"); }</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1">
+    <row r="145" spans="1:8">
       <c r="A145">
         <f t="shared" si="11"/>
         <v>193</v>
@@ -10355,7 +10387,7 @@
         <v>@Test public void testConvert_193() throws Exception { verify( (char) 193, "Á"); }</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1">
+    <row r="146" spans="1:8">
       <c r="A146">
         <f t="shared" si="11"/>
         <v>194</v>
@@ -10381,7 +10413,7 @@
         <v>@Test public void testConvert_194() throws Exception { verify( (char) 194, "Â"); }</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1">
+    <row r="147" spans="1:8">
       <c r="A147">
         <f t="shared" si="11"/>
         <v>195</v>
@@ -10407,7 +10439,7 @@
         <v>@Test public void testConvert_195() throws Exception { verify( (char) 195, "Ã"); }</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1">
+    <row r="148" spans="1:8">
       <c r="A148">
         <f t="shared" si="11"/>
         <v>196</v>
@@ -10433,7 +10465,7 @@
         <v>@Test public void testConvert_196() throws Exception { verify( (char) 196, "Ä"); }</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1">
+    <row r="149" spans="1:8">
       <c r="A149">
         <f t="shared" si="11"/>
         <v>197</v>
@@ -10459,7 +10491,7 @@
         <v>@Test public void testConvert_197() throws Exception { verify( (char) 197, "Å"); }</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1">
+    <row r="150" spans="1:8">
       <c r="A150">
         <f t="shared" si="11"/>
         <v>198</v>
@@ -10485,7 +10517,7 @@
         <v>@Test public void testConvert_198() throws Exception { verify( (char) 198, "Æ"); }</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1">
+    <row r="151" spans="1:8">
       <c r="A151">
         <f t="shared" si="11"/>
         <v>199</v>
@@ -10511,7 +10543,7 @@
         <v>@Test public void testConvert_199() throws Exception { verify( (char) 199, "Ç"); }</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1">
+    <row r="152" spans="1:8">
       <c r="A152">
         <f t="shared" si="11"/>
         <v>200</v>
@@ -10537,7 +10569,7 @@
         <v>@Test public void testConvert_200() throws Exception { verify( (char) 200, "È"); }</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1">
+    <row r="153" spans="1:8">
       <c r="A153">
         <f t="shared" si="11"/>
         <v>201</v>
@@ -10563,7 +10595,7 @@
         <v>@Test public void testConvert_201() throws Exception { verify( (char) 201, "É"); }</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1">
+    <row r="154" spans="1:8">
       <c r="A154">
         <f t="shared" si="11"/>
         <v>202</v>
@@ -10589,7 +10621,7 @@
         <v>@Test public void testConvert_202() throws Exception { verify( (char) 202, "Ê"); }</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1">
+    <row r="155" spans="1:8">
       <c r="A155">
         <f t="shared" si="11"/>
         <v>203</v>
@@ -10615,7 +10647,7 @@
         <v>@Test public void testConvert_203() throws Exception { verify( (char) 203, "Ë"); }</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1">
+    <row r="156" spans="1:8">
       <c r="A156">
         <f t="shared" si="11"/>
         <v>204</v>
@@ -10667,7 +10699,7 @@
         <v>@Test public void testConvert_205() throws Exception { verify( (char) 205, "Í"); }</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1">
+    <row r="158" spans="1:8">
       <c r="A158">
         <f t="shared" si="11"/>
         <v>206</v>
@@ -10693,7 +10725,7 @@
         <v>@Test public void testConvert_206() throws Exception { verify( (char) 206, "Î"); }</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1">
+    <row r="159" spans="1:8">
       <c r="A159">
         <f t="shared" si="11"/>
         <v>207</v>
@@ -10745,7 +10777,7 @@
         <v>@Test public void testConvert_208() throws Exception { verify( (char) 208, "Ð"); }</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1">
+    <row r="161" spans="1:8">
       <c r="A161">
         <f t="shared" si="11"/>
         <v>209</v>
@@ -10797,7 +10829,7 @@
         <v>@Test public void testConvert_210() throws Exception { verify( (char) 210, "Ò"); }</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1">
+    <row r="163" spans="1:8">
       <c r="A163">
         <f t="shared" si="11"/>
         <v>211</v>
@@ -10823,7 +10855,7 @@
         <v>@Test public void testConvert_211() throws Exception { verify( (char) 211, "Ó"); }</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1">
+    <row r="164" spans="1:8">
       <c r="A164">
         <f t="shared" si="11"/>
         <v>212</v>
@@ -10849,7 +10881,7 @@
         <v>@Test public void testConvert_212() throws Exception { verify( (char) 212, "Ô"); }</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1">
+    <row r="165" spans="1:8">
       <c r="A165">
         <f t="shared" si="11"/>
         <v>213</v>
@@ -10875,7 +10907,7 @@
         <v>@Test public void testConvert_213() throws Exception { verify( (char) 213, "Õ"); }</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1">
+    <row r="166" spans="1:8">
       <c r="A166">
         <f t="shared" si="11"/>
         <v>214</v>
@@ -10927,7 +10959,7 @@
         <v>@Test public void testConvert_215() throws Exception { verify( (char) 215, "×"); }</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1">
+    <row r="168" spans="1:8">
       <c r="A168">
         <f t="shared" si="11"/>
         <v>216</v>
@@ -10953,7 +10985,7 @@
         <v>@Test public void testConvert_216() throws Exception { verify( (char) 216, "Ø"); }</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1">
+    <row r="169" spans="1:8">
       <c r="A169">
         <f t="shared" si="11"/>
         <v>217</v>
@@ -10979,7 +11011,7 @@
         <v>@Test public void testConvert_217() throws Exception { verify( (char) 217, "Ù"); }</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1">
+    <row r="170" spans="1:8">
       <c r="A170">
         <f t="shared" si="11"/>
         <v>218</v>
@@ -11031,7 +11063,7 @@
         <v>@Test public void testConvert_219() throws Exception { verify( (char) 219, "Û"); }</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1">
+    <row r="172" spans="1:8">
       <c r="A172">
         <f t="shared" si="11"/>
         <v>220</v>
@@ -11057,7 +11089,7 @@
         <v>@Test public void testConvert_220() throws Exception { verify( (char) 220, "Ü"); }</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1">
+    <row r="173" spans="1:8">
       <c r="A173">
         <f t="shared" si="11"/>
         <v>221</v>
@@ -11109,7 +11141,7 @@
         <v>@Test public void testConvert_222() throws Exception { verify( (char) 222, "Þ"); }</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1">
+    <row r="175" spans="1:8">
       <c r="A175">
         <f t="shared" ref="A175:A207" si="14">HEX2DEC(MID(B175,3,4))</f>
         <v>223</v>
@@ -11135,7 +11167,7 @@
         <v>@Test public void testConvert_223() throws Exception { verify( (char) 223, "ß"); }</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1">
+    <row r="176" spans="1:8">
       <c r="A176">
         <f t="shared" si="14"/>
         <v>224</v>
@@ -11161,7 +11193,7 @@
         <v>@Test public void testConvert_224() throws Exception { verify( (char) 224, "à"); }</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1">
+    <row r="177" spans="1:8">
       <c r="A177">
         <f t="shared" si="14"/>
         <v>225</v>
@@ -11242,7 +11274,7 @@
         <v>@Test public void testConvert_227() throws Exception { verify( (char) 227, "ã"); }</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1">
+    <row r="180" spans="1:8">
       <c r="A180">
         <f t="shared" si="14"/>
         <v>228</v>
@@ -11294,7 +11326,7 @@
         <v>@Test public void testConvert_229() throws Exception { verify( (char) 229, "å"); }</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1">
+    <row r="182" spans="1:8">
       <c r="A182">
         <f t="shared" si="14"/>
         <v>230</v>
@@ -11320,7 +11352,7 @@
         <v>@Test public void testConvert_230() throws Exception { verify( (char) 230, "æ"); }</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1">
+    <row r="183" spans="1:8">
       <c r="A183">
         <f t="shared" si="14"/>
         <v>231</v>
@@ -11346,7 +11378,7 @@
         <v>@Test public void testConvert_231() throws Exception { verify( (char) 231, "ç"); }</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1">
+    <row r="184" spans="1:8">
       <c r="A184">
         <f t="shared" si="14"/>
         <v>232</v>
@@ -11372,7 +11404,7 @@
         <v>@Test public void testConvert_232() throws Exception { verify( (char) 232, "è"); }</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1">
+    <row r="185" spans="1:8">
       <c r="A185">
         <f t="shared" si="14"/>
         <v>233</v>
@@ -11398,7 +11430,7 @@
         <v>@Test public void testConvert_233() throws Exception { verify( (char) 233, "é"); }</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1">
+    <row r="186" spans="1:8">
       <c r="A186">
         <f t="shared" si="14"/>
         <v>234</v>
@@ -11450,7 +11482,7 @@
         <v>@Test public void testConvert_235() throws Exception { verify( (char) 235, "ë"); }</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1">
+    <row r="188" spans="1:8">
       <c r="A188">
         <f t="shared" si="14"/>
         <v>236</v>
@@ -11476,7 +11508,7 @@
         <v>@Test public void testConvert_236() throws Exception { verify( (char) 236, "ì"); }</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1">
+    <row r="189" spans="1:8">
       <c r="A189">
         <f t="shared" si="14"/>
         <v>237</v>
@@ -11502,7 +11534,7 @@
         <v>@Test public void testConvert_237() throws Exception { verify( (char) 237, "í"); }</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1">
+    <row r="190" spans="1:8">
       <c r="A190">
         <f t="shared" si="14"/>
         <v>238</v>
@@ -11528,7 +11560,7 @@
         <v>@Test public void testConvert_238() throws Exception { verify( (char) 238, "î"); }</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1">
+    <row r="191" spans="1:8">
       <c r="A191">
         <f t="shared" si="14"/>
         <v>239</v>
@@ -11554,7 +11586,7 @@
         <v>@Test public void testConvert_239() throws Exception { verify( (char) 239, "ï"); }</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1">
+    <row r="192" spans="1:8">
       <c r="A192">
         <f t="shared" si="14"/>
         <v>240</v>
@@ -11580,7 +11612,7 @@
         <v>@Test public void testConvert_240() throws Exception { verify( (char) 240, "ð"); }</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1">
+    <row r="193" spans="1:8">
       <c r="A193">
         <f t="shared" si="14"/>
         <v>241</v>
@@ -11606,7 +11638,7 @@
         <v>@Test public void testConvert_241() throws Exception { verify( (char) 241, "ñ"); }</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1">
+    <row r="194" spans="1:8">
       <c r="A194">
         <f t="shared" si="14"/>
         <v>242</v>
@@ -11632,7 +11664,7 @@
         <v>@Test public void testConvert_242() throws Exception { verify( (char) 242, "ò"); }</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1">
+    <row r="195" spans="1:8">
       <c r="A195">
         <f t="shared" si="14"/>
         <v>243</v>
@@ -11658,7 +11690,7 @@
         <v>@Test public void testConvert_243() throws Exception { verify( (char) 243, "ó"); }</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1">
+    <row r="196" spans="1:8">
       <c r="A196">
         <f t="shared" si="14"/>
         <v>244</v>
@@ -11684,7 +11716,7 @@
         <v>@Test public void testConvert_244() throws Exception { verify( (char) 244, "ô"); }</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1">
+    <row r="197" spans="1:8">
       <c r="A197">
         <f t="shared" si="14"/>
         <v>245</v>
@@ -11710,7 +11742,7 @@
         <v>@Test public void testConvert_245() throws Exception { verify( (char) 245, "õ"); }</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1">
+    <row r="198" spans="1:8">
       <c r="A198">
         <f t="shared" si="14"/>
         <v>246</v>
@@ -11736,7 +11768,7 @@
         <v>@Test public void testConvert_246() throws Exception { verify( (char) 246, "ö"); }</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1">
+    <row r="199" spans="1:8">
       <c r="A199">
         <f t="shared" si="14"/>
         <v>247</v>
@@ -11762,7 +11794,7 @@
         <v>@Test public void testConvert_247() throws Exception { verify( (char) 247, "÷"); }</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1">
+    <row r="200" spans="1:8">
       <c r="A200">
         <f t="shared" si="14"/>
         <v>248</v>
@@ -11788,7 +11820,7 @@
         <v>@Test public void testConvert_248() throws Exception { verify( (char) 248, "ø"); }</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1">
+    <row r="201" spans="1:8">
       <c r="A201">
         <f t="shared" si="14"/>
         <v>249</v>
@@ -11814,7 +11846,7 @@
         <v>@Test public void testConvert_249() throws Exception { verify( (char) 249, "ù"); }</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1">
+    <row r="202" spans="1:8">
       <c r="A202">
         <f t="shared" si="14"/>
         <v>250</v>
@@ -11840,7 +11872,7 @@
         <v>@Test public void testConvert_250() throws Exception { verify( (char) 250, "ú"); }</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1">
+    <row r="203" spans="1:8">
       <c r="A203">
         <f t="shared" si="14"/>
         <v>251</v>
@@ -11866,7 +11898,7 @@
         <v>@Test public void testConvert_251() throws Exception { verify( (char) 251, "û"); }</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1">
+    <row r="204" spans="1:8">
       <c r="A204">
         <f t="shared" si="14"/>
         <v>252</v>
@@ -11892,7 +11924,7 @@
         <v>@Test public void testConvert_252() throws Exception { verify( (char) 252, "ü"); }</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1">
+    <row r="205" spans="1:8">
       <c r="A205">
         <f t="shared" si="14"/>
         <v>253</v>
@@ -11918,7 +11950,7 @@
         <v>@Test public void testConvert_253() throws Exception { verify( (char) 253, "ý"); }</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1">
+    <row r="206" spans="1:8">
       <c r="A206">
         <f t="shared" si="14"/>
         <v>254</v>
@@ -11944,7 +11976,7 @@
         <v>@Test public void testConvert_254() throws Exception { verify( (char) 254, "þ"); }</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1">
+    <row r="207" spans="1:8">
       <c r="A207">
         <f t="shared" si="14"/>
         <v>255</v>
@@ -11970,13 +12002,34 @@
         <v>@Test public void testConvert_255() throws Exception { verify( (char) 255, "ÿ"); }</v>
       </c>
     </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="26" t="s">
+        <v>854</v>
+      </c>
+      <c r="B211" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="29" t="s">
+        <v>854</v>
+      </c>
+      <c r="B212" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="28" t="s">
+        <v>854</v>
+      </c>
+      <c r="B213" t="s">
+        <v>857</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:E207">
-    <filterColumn colId="1">
+    <filterColumn colId="3">
       <colorFilter dxfId="0" cellColor="0"/>
-    </filterColumn>
-    <filterColumn colId="3">
-      <colorFilter dxfId="1" cellColor="0"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>